<commit_message>
added aurora post flight plots
</commit_message>
<xml_diff>
--- a/analysis/aurora/aurora_flight_data.xlsx
+++ b/analysis/aurora/aurora_flight_data.xlsx
@@ -10,6 +10,7 @@
     <sheet name="proc_cmd" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="mcb_encoder" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="state_est_data" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="altimu_meas" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -39,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -52,6 +53,27 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -54611,7 +54633,6 @@
           <t>STATE_ID_RATE_WX</t>
         </is>
       </c>
-      <c r="C162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="n">
@@ -54622,7 +54643,6 @@
           <t>STATE_ID_RATE_WY</t>
         </is>
       </c>
-      <c r="C163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -54633,7 +54653,6 @@
           <t>STATE_ID_RATE_WZ</t>
         </is>
       </c>
-      <c r="C164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -54644,7 +54663,6 @@
           <t>STATE_ID_VEL_VX</t>
         </is>
       </c>
-      <c r="C165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -54655,7 +54673,6 @@
           <t>STATE_ID_VEL_VY</t>
         </is>
       </c>
-      <c r="C166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -54666,7 +54683,6 @@
           <t>STATE_ID_VEL_VZ</t>
         </is>
       </c>
-      <c r="C167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -54677,7 +54693,6 @@
           <t>STATE_ID_ALT</t>
         </is>
       </c>
-      <c r="C168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -54688,7 +54703,6 @@
           <t>STATE_ID_COEFF_CL</t>
         </is>
       </c>
-      <c r="C169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -54699,9 +54713,777 @@
           <t>STATE_ID_CANARD_ANGLE</t>
         </is>
       </c>
-      <c r="C170" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="1" t="n"/>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="n"/>
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="n"/>
+      <c r="I1" s="1" t="n"/>
+      <c r="J1" s="1" t="n"/>
+      <c r="K1" s="1" t="n"/>
+      <c r="L1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>time_ms</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>pressure</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>temp</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>vel_x</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>accel_x</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>vel_y</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>accel_y</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>vel_z</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>accel_z</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>mag_x</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>mag_y</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>mag_z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>24712</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2213225</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3226</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3996</v>
+      </c>
+      <c r="I3" t="n">
+        <v>7686</v>
+      </c>
+      <c r="J3" t="n">
+        <v>64871</v>
+      </c>
+      <c r="K3" t="n">
+        <v>906</v>
+      </c>
+      <c r="L3" t="n">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>25029</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2175746</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3211</v>
+      </c>
+      <c r="D4" t="n">
+        <v>69</v>
+      </c>
+      <c r="E4" t="n">
+        <v>63812</v>
+      </c>
+      <c r="F4" t="n">
+        <v>582</v>
+      </c>
+      <c r="G4" t="n">
+        <v>654</v>
+      </c>
+      <c r="H4" t="n">
+        <v>4564</v>
+      </c>
+      <c r="I4" t="n">
+        <v>7823</v>
+      </c>
+      <c r="J4" t="n">
+        <v>64335</v>
+      </c>
+      <c r="K4" t="n">
+        <v>502</v>
+      </c>
+      <c r="L4" t="n">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>39917</v>
+      </c>
+      <c r="D5" t="n">
+        <v>27</v>
+      </c>
+      <c r="E5" t="n">
+        <v>65499</v>
+      </c>
+      <c r="F5" t="n">
+        <v>65493</v>
+      </c>
+      <c r="G5" t="n">
+        <v>21</v>
+      </c>
+      <c r="H5" t="n">
+        <v>64884</v>
+      </c>
+      <c r="I5" t="n">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>40237</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1115428</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3258</v>
+      </c>
+      <c r="D6" t="n">
+        <v>65535</v>
+      </c>
+      <c r="E6" t="n">
+        <v>65500</v>
+      </c>
+      <c r="F6" t="n">
+        <v>44</v>
+      </c>
+      <c r="G6" t="n">
+        <v>65423</v>
+      </c>
+      <c r="H6" t="n">
+        <v>65018</v>
+      </c>
+      <c r="I6" t="n">
+        <v>750</v>
+      </c>
+      <c r="J6" t="n">
+        <v>63952</v>
+      </c>
+      <c r="K6" t="n">
+        <v>924</v>
+      </c>
+      <c r="L6" t="n">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>55125</v>
+      </c>
+      <c r="B7" t="n">
+        <v>819957</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3245</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>55229</v>
+      </c>
+      <c r="D8" t="n">
+        <v>65522</v>
+      </c>
+      <c r="E8" t="n">
+        <v>65510</v>
+      </c>
+      <c r="F8" t="n">
+        <v>65477</v>
+      </c>
+      <c r="G8" t="n">
+        <v>65532</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1089</v>
+      </c>
+      <c r="I8" t="n">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>55440</v>
+      </c>
+      <c r="B9" t="n">
+        <v>818682</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3245</v>
+      </c>
+      <c r="D9" t="n">
+        <v>65519</v>
+      </c>
+      <c r="E9" t="n">
+        <v>65477</v>
+      </c>
+      <c r="F9" t="n">
+        <v>65491</v>
+      </c>
+      <c r="G9" t="n">
+        <v>65520</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1155</v>
+      </c>
+      <c r="I9" t="n">
+        <v>159</v>
+      </c>
+      <c r="J9" t="n">
+        <v>65174</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1232</v>
+      </c>
+      <c r="L9" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>55546</v>
+      </c>
+      <c r="D10" t="n">
+        <v>65516</v>
+      </c>
+      <c r="E10" t="n">
+        <v>65506</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>70327</v>
+      </c>
+      <c r="B11" t="n">
+        <v>799316</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3141</v>
+      </c>
+      <c r="D11" t="n">
+        <v>22</v>
+      </c>
+      <c r="E11" t="n">
+        <v>15</v>
+      </c>
+      <c r="F11" t="n">
+        <v>65475</v>
+      </c>
+      <c r="G11" t="n">
+        <v>100</v>
+      </c>
+      <c r="H11" t="n">
+        <v>649</v>
+      </c>
+      <c r="I11" t="n">
+        <v>313</v>
+      </c>
+      <c r="J11" t="n">
+        <v>64857</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1531</v>
+      </c>
+      <c r="L11" t="n">
+        <v>65194</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>85426</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1019289</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2806</v>
+      </c>
+      <c r="F12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G12" t="n">
+        <v>65137</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1094</v>
+      </c>
+      <c r="I12" t="n">
+        <v>905</v>
+      </c>
+      <c r="J12" t="n">
+        <v>64876</v>
+      </c>
+      <c r="K12" t="n">
+        <v>824</v>
+      </c>
+      <c r="L12" t="n">
+        <v>64868</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>85532</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1016676</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2804</v>
+      </c>
+      <c r="D13" t="n">
+        <v>65514</v>
+      </c>
+      <c r="E13" t="n">
+        <v>65484</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" t="n">
+        <v>24</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1053</v>
+      </c>
+      <c r="I13" t="n">
+        <v>940</v>
+      </c>
+      <c r="J13" t="n">
+        <v>64862</v>
+      </c>
+      <c r="K13" t="n">
+        <v>771</v>
+      </c>
+      <c r="L13" t="n">
+        <v>64853</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>85743</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1027103</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2803</v>
+      </c>
+      <c r="D14" t="n">
+        <v>65508</v>
+      </c>
+      <c r="E14" t="n">
+        <v>65447</v>
+      </c>
+      <c r="F14" t="n">
+        <v>65526</v>
+      </c>
+      <c r="G14" t="n">
+        <v>65272</v>
+      </c>
+      <c r="H14" t="n">
+        <v>919</v>
+      </c>
+      <c r="I14" t="n">
+        <v>905</v>
+      </c>
+      <c r="J14" t="n">
+        <v>64823</v>
+      </c>
+      <c r="K14" t="n">
+        <v>688</v>
+      </c>
+      <c r="L14" t="n">
+        <v>64854</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>100738</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1487106</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2313</v>
+      </c>
+      <c r="F15" t="n">
+        <v>17</v>
+      </c>
+      <c r="G15" t="n">
+        <v>65202</v>
+      </c>
+      <c r="H15" t="n">
+        <v>6</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1792</v>
+      </c>
+      <c r="J15" t="n">
+        <v>64201</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1013</v>
+      </c>
+      <c r="L15" t="n">
+        <v>64799</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>100950</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1494342</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2308</v>
+      </c>
+      <c r="D16" t="n">
+        <v>30</v>
+      </c>
+      <c r="E16" t="n">
+        <v>79</v>
+      </c>
+      <c r="F16" t="n">
+        <v>9</v>
+      </c>
+      <c r="G16" t="n">
+        <v>65403</v>
+      </c>
+      <c r="H16" t="n">
+        <v>116</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1892</v>
+      </c>
+      <c r="J16" t="n">
+        <v>64220</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1003</v>
+      </c>
+      <c r="L16" t="n">
+        <v>64664</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>115945</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2161418</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2105</v>
+      </c>
+      <c r="H17" t="n">
+        <v>64991</v>
+      </c>
+      <c r="I17" t="n">
+        <v>2021</v>
+      </c>
+      <c r="J17" t="n">
+        <v>64393</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1087</v>
+      </c>
+      <c r="L17" t="n">
+        <v>64771</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>116260</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2158255</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2106</v>
+      </c>
+      <c r="D18" t="n">
+        <v>61</v>
+      </c>
+      <c r="E18" t="n">
+        <v>64950</v>
+      </c>
+      <c r="F18" t="n">
+        <v>65475</v>
+      </c>
+      <c r="G18" t="n">
+        <v>65421</v>
+      </c>
+      <c r="H18" t="n">
+        <v>64988</v>
+      </c>
+      <c r="I18" t="n">
+        <v>2146</v>
+      </c>
+      <c r="J18" t="n">
+        <v>64367</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1084</v>
+      </c>
+      <c r="L18" t="n">
+        <v>64759</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>116366</v>
+      </c>
+      <c r="D19" t="n">
+        <v>24</v>
+      </c>
+      <c r="E19" t="n">
+        <v>64644</v>
+      </c>
+      <c r="F19" t="n">
+        <v>65531</v>
+      </c>
+      <c r="G19" t="n">
+        <v>31</v>
+      </c>
+      <c r="H19" t="n">
+        <v>64817</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2256</v>
+      </c>
+      <c r="J19" t="n">
+        <v>64359</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>131253</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2977769</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2088</v>
+      </c>
+      <c r="D20" t="n">
+        <v>57</v>
+      </c>
+      <c r="E20" t="n">
+        <v>64640</v>
+      </c>
+      <c r="F20" t="n">
+        <v>65535</v>
+      </c>
+      <c r="G20" t="n">
+        <v>65244</v>
+      </c>
+      <c r="H20" t="n">
+        <v>63759</v>
+      </c>
+      <c r="I20" t="n">
+        <v>2266</v>
+      </c>
+      <c r="J20" t="n">
+        <v>64641</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1118</v>
+      </c>
+      <c r="L20" t="n">
+        <v>64793</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>131569</v>
+      </c>
+      <c r="D21" t="n">
+        <v>52</v>
+      </c>
+      <c r="E21" t="n">
+        <v>65063</v>
+      </c>
+      <c r="F21" t="n">
+        <v>96</v>
+      </c>
+      <c r="G21" t="n">
+        <v>104</v>
+      </c>
+      <c r="H21" t="n">
+        <v>63520</v>
+      </c>
+      <c r="I21" t="n">
+        <v>2461</v>
+      </c>
+      <c r="J21" t="n">
+        <v>64425</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1136</v>
+      </c>
+      <c r="L21" t="n">
+        <v>64790</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>146457</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3912278</v>
+      </c>
+      <c r="C22" t="n">
+        <v>2174</v>
+      </c>
+      <c r="D22" t="n">
+        <v>65469</v>
+      </c>
+      <c r="E22" t="n">
+        <v>65062</v>
+      </c>
+      <c r="F22" t="n">
+        <v>118</v>
+      </c>
+      <c r="G22" t="n">
+        <v>65304</v>
+      </c>
+      <c r="H22" t="n">
+        <v>64204</v>
+      </c>
+      <c r="I22" t="n">
+        <v>2241</v>
+      </c>
+      <c r="J22" t="n">
+        <v>64209</v>
+      </c>
+      <c r="K22" t="n">
+        <v>918</v>
+      </c>
+      <c r="L22" t="n">
+        <v>64761</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>146563</v>
+      </c>
+      <c r="D23" t="n">
+        <v>446</v>
+      </c>
+      <c r="E23" t="n">
+        <v>65401</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>146774</v>
+      </c>
+      <c r="D24" t="n">
+        <v>45</v>
+      </c>
+      <c r="E24" t="n">
+        <v>54</v>
+      </c>
+      <c r="F24" t="n">
+        <v>48</v>
+      </c>
+      <c r="G24" t="n">
+        <v>64657</v>
+      </c>
+      <c r="H24" t="n">
+        <v>64365</v>
+      </c>
+      <c r="I24" t="n">
+        <v>2550</v>
+      </c>
+      <c r="J24" t="n">
+        <v>64196</v>
+      </c>
+      <c r="K24" t="n">
+        <v>789</v>
+      </c>
+      <c r="L24" t="n">
+        <v>64752</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>